<commit_message>
ok for real this time, updated icd2
</commit_message>
<xml_diff>
--- a/icd_compare/mapping_template.xlsx
+++ b/icd_compare/mapping_template.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Columns" sheetId="1" r:id="rId1"/>
     <sheet name="Instructions" sheetId="2" r:id="rId2"/>
+    <sheet name="ValidationLists" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>left_column</t>
   </si>
@@ -32,25 +33,52 @@
     <t>fill_down</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Subcategory</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
     <t>Value</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
     <t>Action</t>
+  </si>
+  <si>
+    <t>Step 1</t>
+  </si>
+  <si>
+    <t>Step 2</t>
+  </si>
+  <si>
+    <t>Step 3</t>
+  </si>
+  <si>
+    <t>Step 4</t>
+  </si>
+  <si>
+    <t>Step 5</t>
+  </si>
+  <si>
+    <t>Step 6</t>
+  </si>
+  <si>
+    <t>Review the 'Columns' sheet.</t>
+  </si>
+  <si>
+    <t>Verify 'confirmed_right_column' matches the correct column in the Right file. Clear it if you don't want to compare that column.</t>
+  </si>
+  <si>
+    <t>Mark Key columns by entering 'Y' in 'is_key'. Keys are used to join rows.</t>
+  </si>
+  <si>
+    <t>Mark columns that need Forward Fill (e.g. parent IDs) by entering 'Y' in 'fill_down'. This fills empty cells with the value from the row above.</t>
+  </si>
+  <si>
+    <t>Save this workbook.</t>
+  </si>
+  <si>
+    <t>Run the diff script again with --mapping-confirmed.</t>
   </si>
 </sst>
 </file>
@@ -408,11 +436,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -441,9 +474,6 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -455,43 +485,26 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3">
+      <formula1>ValidationLists!$A$1:$A$2</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -499,10 +512,81 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>